<commit_message>
chenged CSContent in Log function
</commit_message>
<xml_diff>
--- a/SQLScript/Logfile_info.xlsx
+++ b/SQLScript/Logfile_info.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="285">
   <si>
     <t>csmethod</t>
   </si>
@@ -495,9 +495,6 @@
     <t>GetSubcategoryBySID_XML_QS</t>
   </si>
   <si>
-    <t>"subcategory under tid"</t>
-  </si>
-  <si>
     <t>GetSubcategoryByTopID_QS</t>
   </si>
   <si>
@@ -603,9 +600,6 @@
     <t>GetAllCitis_XML_QS</t>
   </si>
   <si>
-    <t>"cities of "+pid</t>
-  </si>
-  <si>
     <t>GetCityByProvince_QS</t>
   </si>
   <si>
@@ -642,9 +636,6 @@
     <t>GetResourcesByID_QS</t>
   </si>
   <si>
-    <t>"resource by lang"</t>
-  </si>
-  <si>
     <t>GetAllResourcesByLang_QS</t>
   </si>
   <si>
@@ -753,9 +744,6 @@
     <t>GetAllGoogleCitis_XML</t>
   </si>
   <si>
-    <t>"cities in"</t>
-  </si>
-  <si>
     <t>GetGoogleCityByProvinceID_QS</t>
   </si>
   <si>
@@ -765,9 +753,6 @@
     <t>GetGoogleCityByProvince_XML_QS</t>
   </si>
   <si>
-    <t>"this city"</t>
-  </si>
-  <si>
     <t>GetGoogleCityByCid_QS</t>
   </si>
   <si>
@@ -789,9 +774,6 @@
     <t>GetAllResourcesByProvince</t>
   </si>
   <si>
-    <t>"in Province"</t>
-  </si>
-  <si>
     <t>GetAllResourcesByProvince_QS</t>
   </si>
   <si>
@@ -804,9 +786,6 @@
     <t>"subcategory"</t>
   </si>
   <si>
-    <t>"in subcategory"</t>
-  </si>
-  <si>
     <t>GetAllResourcesBySubCategory_QS</t>
   </si>
   <si>
@@ -819,9 +798,6 @@
     <t>GetAllResourcesByTopCategory</t>
   </si>
   <si>
-    <t>"in topcategory"</t>
-  </si>
-  <si>
     <t>GetAllResourcesByTopCategory_QS</t>
   </si>
   <si>
@@ -925,6 +901,9 @@
   </si>
   <si>
     <t>IncrementSuggestionWordList_XML_QS</t>
+  </si>
+  <si>
+    <t>"Provincal"</t>
   </si>
 </sst>
 </file>
@@ -1315,13 +1294,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T200"/>
+  <dimension ref="A1:T165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B177" sqref="B177"/>
+      <selection pane="bottomRight" activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1334,8 +1313,9 @@
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
     <col min="12" max="12" width="3" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="3.42578125" hidden="1" customWidth="1"/>
@@ -2164,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>140</v>
@@ -2177,12 +2157,12 @@
       </c>
       <c r="R23" t="str">
         <f t="shared" si="2"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "subcategory under tid"  ,  "subCategory"  ,  tid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "TopCategory"  ,  "subCategory"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="6" customFormat="1">
       <c r="B24" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s">
         <v>109</v>
@@ -2200,7 +2180,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>140</v>
@@ -2213,12 +2193,12 @@
       </c>
       <c r="R24" t="str">
         <f t="shared" si="2"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "subcategory under tid"  ,  "subCategory"  ,  tid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "TopCategory"  ,  "subCategory"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="6" customFormat="1">
       <c r="B25" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
         <v>109</v>
@@ -2236,7 +2216,7 @@
         <v>6</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>140</v>
@@ -2249,12 +2229,12 @@
       </c>
       <c r="R25" t="str">
         <f t="shared" si="2"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "subcategory under tid"  ,  "subCategory"  ,  tid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "TopCategory"  ,  "subCategory"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="6" customFormat="1">
       <c r="B26" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
         <v>109</v>
@@ -2272,7 +2252,7 @@
         <v>6</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>140</v>
@@ -2285,18 +2265,18 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" si="2"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "subcategory under tid"  ,  "subCategory"  ,  tid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "TopCategory"  ,  "subCategory"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="6" customFormat="1">
       <c r="A27" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>130</v>
@@ -2314,7 +2294,7 @@
         <v>104</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>83</v>
@@ -2329,10 +2309,10 @@
     </row>
     <row r="28" spans="1:18" s="6" customFormat="1">
       <c r="B28" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>130</v>
@@ -2350,7 +2330,7 @@
         <v>104</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>83</v>
@@ -2365,10 +2345,10 @@
     </row>
     <row r="29" spans="1:18" s="6" customFormat="1">
       <c r="B29" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>129</v>
@@ -2386,7 +2366,7 @@
         <v>104</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>83</v>
@@ -2401,10 +2381,10 @@
     </row>
     <row r="30" spans="1:18" s="6" customFormat="1">
       <c r="B30" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>129</v>
@@ -2422,7 +2402,7 @@
         <v>104</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>83</v>
@@ -2437,10 +2417,10 @@
     </row>
     <row r="31" spans="1:18" s="6" customFormat="1">
       <c r="A31" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s">
         <v>109</v>
@@ -2476,7 +2456,7 @@
     </row>
     <row r="32" spans="1:18" s="6" customFormat="1">
       <c r="B32" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" t="s">
         <v>109</v>
@@ -2512,7 +2492,7 @@
     </row>
     <row r="33" spans="1:18" s="6" customFormat="1">
       <c r="B33" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
         <v>109</v>
@@ -2548,7 +2528,7 @@
     </row>
     <row r="34" spans="1:18" s="6" customFormat="1">
       <c r="B34" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
         <v>109</v>
@@ -2584,7 +2564,7 @@
     </row>
     <row r="35" spans="1:18" s="6" customFormat="1">
       <c r="B35" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" t="s">
         <v>109</v>
@@ -2620,7 +2600,7 @@
     </row>
     <row r="36" spans="1:18" s="6" customFormat="1">
       <c r="B36" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
         <v>109</v>
@@ -2656,7 +2636,7 @@
     </row>
     <row r="37" spans="1:18" s="6" customFormat="1">
       <c r="B37" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C37" t="s">
         <v>109</v>
@@ -2692,7 +2672,7 @@
     </row>
     <row r="38" spans="1:18" s="6" customFormat="1">
       <c r="B38" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
         <v>109</v>
@@ -2728,7 +2708,7 @@
     </row>
     <row r="39" spans="1:18" s="6" customFormat="1">
       <c r="A39" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>76</v>
@@ -2767,7 +2747,7 @@
     </row>
     <row r="40" spans="1:18">
       <c r="B40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
         <v>109</v>
@@ -2803,7 +2783,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="B41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
         <v>109</v>
@@ -2839,7 +2819,7 @@
     </row>
     <row r="42" spans="1:18">
       <c r="B42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
         <v>109</v>
@@ -2893,7 +2873,7 @@
         <v>6</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>29</v>
@@ -2906,12 +2886,12 @@
       </c>
       <c r="R43" t="str">
         <f t="shared" si="3"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  token  ,  "cities of "+pid  ,  "city"  ,  pid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  token  ,  "Provincal"  ,  "city"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="44" spans="1:18">
       <c r="B44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44" t="s">
         <v>109</v>
@@ -2929,7 +2909,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>29</v>
@@ -2942,12 +2922,12 @@
       </c>
       <c r="R44" t="str">
         <f t="shared" si="3"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  token  ,  "cities of "+pid  ,  "city"  ,  pid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  token  ,  "Provincal"  ,  "city"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="B45" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
         <v>109</v>
@@ -2965,7 +2945,7 @@
         <v>6</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>29</v>
@@ -2978,12 +2958,12 @@
       </c>
       <c r="R45" t="str">
         <f t="shared" si="3"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  token  ,  "cities of "+pid  ,  "city"  ,  pid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  token  ,  "Provincal"  ,  "city"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="B46" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
         <v>109</v>
@@ -3001,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>29</v>
@@ -3014,7 +2994,7 @@
       </c>
       <c r="R46" t="str">
         <f t="shared" si="3"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  token  ,  "cities of "+pid  ,  "city"  ,  pid.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  token  ,  "Provincal"  ,  "city"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="6" customFormat="1">
@@ -3055,7 +3035,7 @@
     </row>
     <row r="48" spans="1:18" s="6" customFormat="1">
       <c r="B48" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
         <v>109</v>
@@ -3091,7 +3071,7 @@
     </row>
     <row r="49" spans="1:18" s="6" customFormat="1">
       <c r="B49" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
         <v>109</v>
@@ -3127,7 +3107,7 @@
     </row>
     <row r="50" spans="1:18" s="6" customFormat="1">
       <c r="B50" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C50" t="s">
         <v>109</v>
@@ -3163,7 +3143,7 @@
     </row>
     <row r="51" spans="1:18" s="6" customFormat="1">
       <c r="B51" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C51" t="s">
         <v>109</v>
@@ -3181,7 +3161,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>29</v>
@@ -3199,7 +3179,7 @@
     </row>
     <row r="52" spans="1:18" s="6" customFormat="1">
       <c r="B52" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C52" t="s">
         <v>109</v>
@@ -3217,7 +3197,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>29</v>
@@ -3235,7 +3215,7 @@
     </row>
     <row r="53" spans="1:18" s="6" customFormat="1">
       <c r="B53" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
         <v>109</v>
@@ -3253,7 +3233,7 @@
         <v>6</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>29</v>
@@ -3271,7 +3251,7 @@
     </row>
     <row r="54" spans="1:18" s="6" customFormat="1">
       <c r="B54" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C54" t="s">
         <v>109</v>
@@ -3289,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>29</v>
@@ -3307,10 +3287,10 @@
     </row>
     <row r="55" spans="1:18" s="6" customFormat="1">
       <c r="A55" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>104</v>
@@ -3319,10 +3299,10 @@
         <v>104</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>104</v>
@@ -3334,7 +3314,7 @@
         <v>87</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>25</v>
@@ -3346,7 +3326,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>104</v>
@@ -3355,7 +3335,7 @@
         <v>104</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G56" t="s">
         <v>1</v>
@@ -3367,10 +3347,10 @@
         <v>90</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K56" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>25</v>
@@ -3382,7 +3362,7 @@
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>104</v>
@@ -3391,7 +3371,7 @@
         <v>104</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G57" t="s">
         <v>1</v>
@@ -3403,10 +3383,10 @@
         <v>90</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K57" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>25</v>
@@ -3418,7 +3398,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>104</v>
@@ -3427,10 +3407,10 @@
         <v>104</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G58" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>104</v>
@@ -3442,7 +3422,7 @@
         <v>95</v>
       </c>
       <c r="K58" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="Q58" s="3" t="s">
         <v>25</v>
@@ -3454,34 +3434,34 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" t="s">
         <v>170</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G59" t="s">
+        <v>179</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I59" t="s">
+        <v>178</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" s="5" t="s">
+      <c r="K59" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G59" t="s">
-        <v>180</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="K59" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="Q59" s="3" t="s">
         <v>25</v>
@@ -3493,34 +3473,34 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" t="s">
+        <v>177</v>
+      </c>
+      <c r="C60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G60" t="s">
+        <v>179</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I60" t="s">
         <v>178</v>
       </c>
-      <c r="B60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C60" t="s">
-        <v>109</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G60" t="s">
-        <v>180</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I60" t="s">
-        <v>179</v>
-      </c>
       <c r="J60" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K60" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>25</v>
@@ -3532,7 +3512,7 @@
     </row>
     <row r="61" spans="1:18" s="6" customFormat="1">
       <c r="A61" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>66</v>
@@ -3571,7 +3551,7 @@
     </row>
     <row r="62" spans="1:18" s="6" customFormat="1">
       <c r="B62" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C62" t="s">
         <v>109</v>
@@ -3625,7 +3605,7 @@
         <v>104</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>67</v>
@@ -3637,13 +3617,13 @@
         <v>25</v>
       </c>
       <c r="R63" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C63&amp;$A$1&amp;E63&amp;$A$1&amp;F63&amp;$A$1&amp;G63&amp;$A$1&amp;H63&amp;$A$1&amp;I63&amp;$A$1&amp;J63&amp;$A$1&amp;K63&amp;Q63</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "cities in"  ,  "google"  ,  pid.ToString());</v>
+        <f t="shared" ref="R63:R74" si="7">"logservices.logservices(request, response"&amp;$A$1&amp;C63&amp;$A$1&amp;E63&amp;$A$1&amp;F63&amp;$A$1&amp;G63&amp;$A$1&amp;H63&amp;$A$1&amp;I63&amp;$A$1&amp;J63&amp;$A$1&amp;K63&amp;Q63</f>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "Provincal"  ,  "google"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="64" spans="1:18">
       <c r="B64" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C64" t="s">
         <v>109</v>
@@ -3661,7 +3641,7 @@
         <v>104</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>67</v>
@@ -3673,13 +3653,13 @@
         <v>25</v>
       </c>
       <c r="R64" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C64&amp;$A$1&amp;E64&amp;$A$1&amp;F64&amp;$A$1&amp;G64&amp;$A$1&amp;H64&amp;$A$1&amp;I64&amp;$A$1&amp;J64&amp;$A$1&amp;K64&amp;Q64</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "cities in"  ,  "google"  ,  pid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "Provincal"  ,  "google"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="65" spans="1:18">
       <c r="B65" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C65" t="s">
         <v>109</v>
@@ -3697,7 +3677,7 @@
         <v>104</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>67</v>
@@ -3709,13 +3689,13 @@
         <v>25</v>
       </c>
       <c r="R65" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C65&amp;$A$1&amp;E65&amp;$A$1&amp;F65&amp;$A$1&amp;G65&amp;$A$1&amp;H65&amp;$A$1&amp;I65&amp;$A$1&amp;J65&amp;$A$1&amp;K65&amp;Q65</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "cities in"  ,  "google"  ,  pid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "Provincal"  ,  "google"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="66" spans="1:18">
       <c r="B66" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C66" t="s">
         <v>109</v>
@@ -3733,7 +3713,7 @@
         <v>104</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>67</v>
@@ -3745,8 +3725,8 @@
         <v>25</v>
       </c>
       <c r="R66" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C66&amp;$A$1&amp;E66&amp;$A$1&amp;F66&amp;$A$1&amp;G66&amp;$A$1&amp;H66&amp;$A$1&amp;I66&amp;$A$1&amp;J66&amp;$A$1&amp;K66&amp;Q66</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "cities in"  ,  "google"  ,  pid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "Provincal"  ,  "google"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -3769,7 +3749,7 @@
         <v>104</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="J67" s="6" t="s">
         <v>67</v>
@@ -3781,13 +3761,13 @@
         <v>25</v>
       </c>
       <c r="R67" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C67&amp;$A$1&amp;E67&amp;$A$1&amp;F67&amp;$A$1&amp;G67&amp;$A$1&amp;H67&amp;$A$1&amp;I67&amp;$A$1&amp;J67&amp;$A$1&amp;K67&amp;Q67</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "this city"  ,  "google"  ,  cid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "this"  ,  "google"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="68" spans="1:18">
       <c r="B68" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C68" t="s">
         <v>109</v>
@@ -3805,7 +3785,7 @@
         <v>104</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>67</v>
@@ -3817,13 +3797,13 @@
         <v>25</v>
       </c>
       <c r="R68" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C68&amp;$A$1&amp;E68&amp;$A$1&amp;F68&amp;$A$1&amp;G68&amp;$A$1&amp;H68&amp;$A$1&amp;I68&amp;$A$1&amp;J68&amp;$A$1&amp;K68&amp;Q68</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "this city"  ,  "google"  ,  cid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "this"  ,  "google"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="69" spans="1:18">
       <c r="B69" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C69" t="s">
         <v>109</v>
@@ -3841,7 +3821,7 @@
         <v>104</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="J69" s="6" t="s">
         <v>67</v>
@@ -3853,13 +3833,13 @@
         <v>25</v>
       </c>
       <c r="R69" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C69&amp;$A$1&amp;E69&amp;$A$1&amp;F69&amp;$A$1&amp;G69&amp;$A$1&amp;H69&amp;$A$1&amp;I69&amp;$A$1&amp;J69&amp;$A$1&amp;K69&amp;Q69</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "this city"  ,  "google"  ,  cid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "this"  ,  "google"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C70" t="s">
         <v>109</v>
@@ -3877,7 +3857,7 @@
         <v>104</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>238</v>
+        <v>116</v>
       </c>
       <c r="J70" s="6" t="s">
         <v>67</v>
@@ -3889,8 +3869,8 @@
         <v>25</v>
       </c>
       <c r="R70" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C70&amp;$A$1&amp;E70&amp;$A$1&amp;F70&amp;$A$1&amp;G70&amp;$A$1&amp;H70&amp;$A$1&amp;I70&amp;$A$1&amp;J70&amp;$A$1&amp;K70&amp;Q70</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "this city"  ,  "google"  ,  cid.ToString());</v>
+        <f t="shared" si="7"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "this"  ,  "google"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="71" spans="1:18">
@@ -3913,7 +3893,7 @@
         <v>104</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>67</v>
@@ -3925,13 +3905,13 @@
         <v>25</v>
       </c>
       <c r="R71" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C71&amp;$A$1&amp;E71&amp;$A$1&amp;F71&amp;$A$1&amp;G71&amp;$A$1&amp;H71&amp;$A$1&amp;I71&amp;$A$1&amp;J71&amp;$A$1&amp;K71&amp;Q71</f>
+        <f t="shared" si="7"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "google"  ,  cl);</v>
       </c>
     </row>
     <row r="72" spans="1:18">
       <c r="B72" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C72" t="s">
         <v>109</v>
@@ -3949,7 +3929,7 @@
         <v>104</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>67</v>
@@ -3961,13 +3941,13 @@
         <v>25</v>
       </c>
       <c r="R72" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C72&amp;$A$1&amp;E72&amp;$A$1&amp;F72&amp;$A$1&amp;G72&amp;$A$1&amp;H72&amp;$A$1&amp;I72&amp;$A$1&amp;J72&amp;$A$1&amp;K72&amp;Q72</f>
+        <f t="shared" si="7"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "google"  ,  cl);</v>
       </c>
     </row>
     <row r="73" spans="1:18">
       <c r="B73" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C73" t="s">
         <v>109</v>
@@ -3985,7 +3965,7 @@
         <v>104</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J73" s="6" t="s">
         <v>67</v>
@@ -3997,13 +3977,13 @@
         <v>25</v>
       </c>
       <c r="R73" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C73&amp;$A$1&amp;E73&amp;$A$1&amp;F73&amp;$A$1&amp;G73&amp;$A$1&amp;H73&amp;$A$1&amp;I73&amp;$A$1&amp;J73&amp;$A$1&amp;K73&amp;Q73</f>
+        <f t="shared" si="7"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "google"  ,  cl);</v>
       </c>
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C74" t="s">
         <v>109</v>
@@ -4021,7 +4001,7 @@
         <v>104</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J74" s="6" t="s">
         <v>67</v>
@@ -4033,7 +4013,7 @@
         <v>25</v>
       </c>
       <c r="R74" t="str">
-        <f>"logservices.logservices(request, response"&amp;$A$1&amp;C74&amp;$A$1&amp;E74&amp;$A$1&amp;F74&amp;$A$1&amp;G74&amp;$A$1&amp;H74&amp;$A$1&amp;I74&amp;$A$1&amp;J74&amp;$A$1&amp;K74&amp;Q74</f>
+        <f t="shared" si="7"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "google"  ,  cl);</v>
       </c>
     </row>
@@ -4060,7 +4040,7 @@
         <v>6</v>
       </c>
       <c r="I75" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="J75" t="s">
         <v>117</v>
@@ -4072,13 +4052,13 @@
         <v>25</v>
       </c>
       <c r="R75" t="str">
-        <f t="shared" ref="R75:R113" si="7">"logservices.logservices(request, response"&amp;$A$1&amp;C75&amp;$A$1&amp;E75&amp;$A$1&amp;F75&amp;$A$1&amp;G75&amp;$A$1&amp;H75&amp;$A$1&amp;I75&amp;$A$1&amp;J75&amp;$A$1&amp;K75&amp;Q75</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "resource by lang"  ,  "resource"  ,  lang);</v>
+        <f t="shared" ref="R75:R113" si="8">"logservices.logservices(request, response"&amp;$A$1&amp;C75&amp;$A$1&amp;E75&amp;$A$1&amp;F75&amp;$A$1&amp;G75&amp;$A$1&amp;H75&amp;$A$1&amp;I75&amp;$A$1&amp;J75&amp;$A$1&amp;K75&amp;Q75</f>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "Language"  ,  "resource"  ,  lang);</v>
       </c>
     </row>
     <row r="76" spans="1:18">
       <c r="B76" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C76" t="s">
         <v>109</v>
@@ -4096,7 +4076,7 @@
         <v>6</v>
       </c>
       <c r="I76" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="J76" t="s">
         <v>117</v>
@@ -4108,13 +4088,13 @@
         <v>25</v>
       </c>
       <c r="R76" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "resource by lang"  ,  "resource"  ,  lang);</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "Language"  ,  "resource"  ,  lang);</v>
       </c>
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C77" t="s">
         <v>109</v>
@@ -4132,7 +4112,7 @@
         <v>6</v>
       </c>
       <c r="I77" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="J77" t="s">
         <v>117</v>
@@ -4144,13 +4124,13 @@
         <v>25</v>
       </c>
       <c r="R77" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "resource by lang"  ,  "resource"  ,  lang);</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "Language"  ,  "resource"  ,  lang);</v>
       </c>
     </row>
     <row r="78" spans="1:18">
       <c r="B78" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C78" t="s">
         <v>109</v>
@@ -4168,7 +4148,7 @@
         <v>6</v>
       </c>
       <c r="I78" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="J78" t="s">
         <v>117</v>
@@ -4180,8 +4160,8 @@
         <v>25</v>
       </c>
       <c r="R78" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "resource by lang"  ,  "resource"  ,  lang);</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "Language"  ,  "resource"  ,  lang);</v>
       </c>
     </row>
     <row r="79" spans="1:18">
@@ -4216,13 +4196,13 @@
         <v>25</v>
       </c>
       <c r="R79" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  token  ,  "all"  ,  "resource"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="B80" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C80" t="s">
         <v>109</v>
@@ -4252,13 +4232,13 @@
         <v>25</v>
       </c>
       <c r="R80" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  token  ,  "all"  ,  "resource"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="81" spans="2:18">
       <c r="B81" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C81" t="s">
         <v>109</v>
@@ -4288,13 +4268,13 @@
         <v>25</v>
       </c>
       <c r="R81" t="str">
-        <f t="shared" ref="R81:R87" si="8">"logservices.logservices(request, response"&amp;$A$1&amp;C81&amp;$A$1&amp;E81&amp;$A$1&amp;F81&amp;$A$1&amp;G81&amp;$A$1&amp;H81&amp;$A$1&amp;I81&amp;$A$1&amp;J81&amp;$A$1&amp;K81&amp;Q81</f>
+        <f t="shared" ref="R81:R87" si="9">"logservices.logservices(request, response"&amp;$A$1&amp;C81&amp;$A$1&amp;E81&amp;$A$1&amp;F81&amp;$A$1&amp;G81&amp;$A$1&amp;H81&amp;$A$1&amp;I81&amp;$A$1&amp;J81&amp;$A$1&amp;K81&amp;Q81</f>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  token  ,  "all"  ,  "resource"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="82" spans="2:18">
       <c r="B82" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
@@ -4324,13 +4304,13 @@
         <v>25</v>
       </c>
       <c r="R82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  token  ,  "all"  ,  "resource"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="83" spans="2:18">
       <c r="B83" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C83" t="s">
         <v>109</v>
@@ -4348,7 +4328,7 @@
         <v>6</v>
       </c>
       <c r="I83" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J83" t="s">
         <v>117</v>
@@ -4360,13 +4340,13 @@
         <v>25</v>
       </c>
       <c r="R83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "type"  ,  "resource"  ,  type);</v>
       </c>
     </row>
     <row r="84" spans="2:18">
       <c r="B84" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C84" t="s">
         <v>109</v>
@@ -4384,7 +4364,7 @@
         <v>6</v>
       </c>
       <c r="I84" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J84" t="s">
         <v>117</v>
@@ -4396,13 +4376,13 @@
         <v>25</v>
       </c>
       <c r="R84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "type"  ,  "resource"  ,  type);</v>
       </c>
     </row>
     <row r="85" spans="2:18">
       <c r="B85" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C85" t="s">
         <v>109</v>
@@ -4420,7 +4400,7 @@
         <v>6</v>
       </c>
       <c r="I85" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J85" t="s">
         <v>117</v>
@@ -4432,13 +4412,13 @@
         <v>25</v>
       </c>
       <c r="R85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "type"  ,  "resource"  ,  type);</v>
       </c>
     </row>
     <row r="86" spans="2:18">
       <c r="B86" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C86" t="s">
         <v>109</v>
@@ -4456,7 +4436,7 @@
         <v>6</v>
       </c>
       <c r="I86" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J86" t="s">
         <v>117</v>
@@ -4468,7 +4448,7 @@
         <v>25</v>
       </c>
       <c r="R86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "type"  ,  "resource"  ,  type);</v>
       </c>
     </row>
@@ -4505,13 +4485,13 @@
         <v>25</v>
       </c>
       <c r="R87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "this"  ,  "resource"  ,  rid.ToString());</v>
       </c>
     </row>
     <row r="88" spans="2:18">
       <c r="B88" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C88" t="s">
         <v>109</v>
@@ -4541,13 +4521,13 @@
         <v>25</v>
       </c>
       <c r="R88" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "this"  ,  "resource"  ,  rid.ToString());</v>
       </c>
     </row>
     <row r="89" spans="2:18">
       <c r="B89" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C89" t="s">
         <v>109</v>
@@ -4583,7 +4563,7 @@
     </row>
     <row r="90" spans="2:18">
       <c r="B90" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
@@ -4613,7 +4593,7 @@
         <v>25</v>
       </c>
       <c r="R90" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "this"  ,  "resource"  ,  rid.ToString());</v>
       </c>
     </row>
@@ -4637,13 +4617,13 @@
         <v>6</v>
       </c>
       <c r="I91" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J91" t="s">
         <v>117</v>
       </c>
       <c r="K91" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>25</v>
@@ -4655,7 +4635,7 @@
     </row>
     <row r="92" spans="2:18">
       <c r="B92" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
@@ -4673,25 +4653,25 @@
         <v>6</v>
       </c>
       <c r="I92" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J92" t="s">
         <v>117</v>
       </c>
       <c r="K92" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R92" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
       </c>
     </row>
     <row r="93" spans="2:18">
       <c r="B93" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
@@ -4709,25 +4689,25 @@
         <v>6</v>
       </c>
       <c r="I93" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J93" t="s">
         <v>117</v>
       </c>
       <c r="K93" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q93" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R93" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
       </c>
     </row>
     <row r="94" spans="2:18">
       <c r="B94" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
@@ -4745,25 +4725,25 @@
         <v>6</v>
       </c>
       <c r="I94" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J94" t="s">
         <v>117</v>
       </c>
       <c r="K94" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Q94" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R94" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
       </c>
     </row>
     <row r="95" spans="2:18">
       <c r="B95" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -4781,7 +4761,7 @@
         <v>6</v>
       </c>
       <c r="I95" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J95" t="s">
         <v>117</v>
@@ -4793,13 +4773,13 @@
         <v>25</v>
       </c>
       <c r="R95" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "in city"  ,  "resource"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="96" spans="2:18">
       <c r="B96" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -4817,7 +4797,7 @@
         <v>6</v>
       </c>
       <c r="I96" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J96" t="s">
         <v>117</v>
@@ -4829,13 +4809,13 @@
         <v>25</v>
       </c>
       <c r="R96" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "in city"  ,  "resource"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="97" spans="2:18">
       <c r="B97" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
@@ -4853,7 +4833,7 @@
         <v>6</v>
       </c>
       <c r="I97" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J97" t="s">
         <v>117</v>
@@ -4865,13 +4845,13 @@
         <v>25</v>
       </c>
       <c r="R97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "in city"  ,  "resource"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="98" spans="2:18">
       <c r="B98" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
@@ -4889,7 +4869,7 @@
         <v>6</v>
       </c>
       <c r="I98" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J98" t="s">
         <v>117</v>
@@ -4901,13 +4881,13 @@
         <v>25</v>
       </c>
       <c r="R98" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "in city"  ,  "resource"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="99" spans="2:18">
       <c r="B99" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
@@ -4925,7 +4905,7 @@
         <v>6</v>
       </c>
       <c r="I99" t="s">
-        <v>246</v>
+        <v>34</v>
       </c>
       <c r="J99" t="s">
         <v>117</v>
@@ -4937,13 +4917,13 @@
         <v>25</v>
       </c>
       <c r="R99" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "in Province"  ,  "resource"  ,  pid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "Province"  ,  "resource"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="100" spans="2:18">
       <c r="B100" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
@@ -4961,7 +4941,7 @@
         <v>6</v>
       </c>
       <c r="I100" t="s">
-        <v>246</v>
+        <v>34</v>
       </c>
       <c r="J100" t="s">
         <v>117</v>
@@ -4973,13 +4953,13 @@
         <v>25</v>
       </c>
       <c r="R100" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "in Province"  ,  "resource"  ,  pid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "Province"  ,  "resource"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="101" spans="2:18">
       <c r="B101" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
@@ -4997,7 +4977,7 @@
         <v>6</v>
       </c>
       <c r="I101" t="s">
-        <v>246</v>
+        <v>34</v>
       </c>
       <c r="J101" t="s">
         <v>117</v>
@@ -5009,13 +4989,13 @@
         <v>25</v>
       </c>
       <c r="R101" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "in Province"  ,  "resource"  ,  pid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "Province"  ,  "resource"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="102" spans="2:18">
       <c r="B102" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
@@ -5033,7 +5013,7 @@
         <v>6</v>
       </c>
       <c r="I102" t="s">
-        <v>246</v>
+        <v>34</v>
       </c>
       <c r="J102" t="s">
         <v>117</v>
@@ -5042,13 +5022,13 @@
         <v>98</v>
       </c>
       <c r="R102" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "in Province"  ,  "resource"  ,  pid.ToString()</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "Province"  ,  "resource"  ,  pid.ToString()</v>
       </c>
     </row>
     <row r="103" spans="2:18">
       <c r="B103" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C103" t="s">
         <v>109</v>
@@ -5066,7 +5046,7 @@
         <v>6</v>
       </c>
       <c r="I103" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="J103" t="s">
         <v>117</v>
@@ -5078,13 +5058,13 @@
         <v>25</v>
       </c>
       <c r="R103" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "in subcategory"  ,  "resource"  ,  sid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "SubCategory"  ,  "resource"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="104" spans="2:18">
       <c r="B104" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
@@ -5102,7 +5082,7 @@
         <v>6</v>
       </c>
       <c r="I104" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="J104" t="s">
         <v>117</v>
@@ -5114,13 +5094,13 @@
         <v>25</v>
       </c>
       <c r="R104" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "in subcategory"  ,  "resource"  ,  sid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "SubCategory"  ,  "resource"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="105" spans="2:18">
       <c r="B105" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C105" t="s">
         <v>109</v>
@@ -5138,7 +5118,7 @@
         <v>6</v>
       </c>
       <c r="I105" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="J105" t="s">
         <v>117</v>
@@ -5150,13 +5130,13 @@
         <v>25</v>
       </c>
       <c r="R105" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "in subcategory"  ,  "resource"  ,  sid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "SubCategory"  ,  "resource"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="106" spans="2:18">
       <c r="B106" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C106" t="s">
         <v>109</v>
@@ -5174,7 +5154,7 @@
         <v>6</v>
       </c>
       <c r="I106" t="s">
-        <v>251</v>
+        <v>16</v>
       </c>
       <c r="J106" t="s">
         <v>117</v>
@@ -5186,13 +5166,13 @@
         <v>25</v>
       </c>
       <c r="R106" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "in subcategory"  ,  "resource"  ,  sid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "SubCategory"  ,  "resource"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="107" spans="2:18">
       <c r="B107" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C107" t="s">
         <v>109</v>
@@ -5210,7 +5190,7 @@
         <v>6</v>
       </c>
       <c r="I107" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J107" t="s">
         <v>117</v>
@@ -5222,13 +5202,13 @@
         <v>25</v>
       </c>
       <c r="R107" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "in topcategory"  ,  "resource"  ,  tid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "TopCategory"  ,  "resource"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="108" spans="2:18">
       <c r="B108" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C108" t="s">
         <v>109</v>
@@ -5246,7 +5226,7 @@
         <v>6</v>
       </c>
       <c r="I108" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J108" t="s">
         <v>117</v>
@@ -5258,13 +5238,13 @@
         <v>25</v>
       </c>
       <c r="R108" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "in topcategory"  ,  "resource"  ,  tid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "TopCategory"  ,  "resource"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="109" spans="2:18">
       <c r="B109" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C109" t="s">
         <v>109</v>
@@ -5282,7 +5262,7 @@
         <v>6</v>
       </c>
       <c r="I109" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J109" t="s">
         <v>117</v>
@@ -5294,13 +5274,13 @@
         <v>25</v>
       </c>
       <c r="R109" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "in topcategory"  ,  "resource"  ,  tid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "TopCategory"  ,  "resource"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="110" spans="2:18">
       <c r="B110" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C110" t="s">
         <v>109</v>
@@ -5318,7 +5298,7 @@
         <v>6</v>
       </c>
       <c r="I110" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J110" t="s">
         <v>117</v>
@@ -5330,13 +5310,13 @@
         <v>25</v>
       </c>
       <c r="R110" t="str">
-        <f t="shared" si="7"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "in topcategory"  ,  "resource"  ,  tid.ToString());</v>
+        <f t="shared" si="8"/>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "TopCategory"  ,  "resource"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="111" spans="2:18">
       <c r="B111" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C111" t="s">
         <v>109</v>
@@ -5360,19 +5340,19 @@
         <v>117</v>
       </c>
       <c r="K111" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q111" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R111" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "search"  ,  "resource"  ,  kws);</v>
       </c>
     </row>
     <row r="112" spans="2:18">
       <c r="B112" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C112" t="s">
         <v>109</v>
@@ -5396,19 +5376,19 @@
         <v>117</v>
       </c>
       <c r="K112" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q112" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R112" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "search"  ,  "resource"  ,  kws);</v>
       </c>
     </row>
     <row r="113" spans="1:18">
       <c r="B113" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C113" t="s">
         <v>109</v>
@@ -5432,19 +5412,19 @@
         <v>117</v>
       </c>
       <c r="K113" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q113" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R113" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "search"  ,  "resource"  ,  kws);</v>
       </c>
     </row>
     <row r="114" spans="1:18">
       <c r="B114" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C114" t="s">
         <v>109</v>
@@ -5468,13 +5448,13 @@
         <v>117</v>
       </c>
       <c r="K114" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q114" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R114" t="str">
-        <f t="shared" ref="R114:R176" si="9">"logservices.logservices(request, response"&amp;$A$1&amp;C114&amp;$A$1&amp;E114&amp;$A$1&amp;F114&amp;$A$1&amp;G114&amp;$A$1&amp;H114&amp;$A$1&amp;I114&amp;$A$1&amp;J114&amp;$A$1&amp;K114&amp;Q114</f>
+        <f t="shared" ref="R114:R164" si="10">"logservices.logservices(request, response"&amp;$A$1&amp;C114&amp;$A$1&amp;E114&amp;$A$1&amp;F114&amp;$A$1&amp;G114&amp;$A$1&amp;H114&amp;$A$1&amp;I114&amp;$A$1&amp;J114&amp;$A$1&amp;K114&amp;Q114</f>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "search"  ,  "resource"  ,  kws);</v>
       </c>
     </row>
@@ -5498,25 +5478,25 @@
         <v>6</v>
       </c>
       <c r="I115" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J115" t="s">
         <v>117</v>
       </c>
       <c r="K115" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q115" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R115" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="116" spans="1:18">
       <c r="B116" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C116" t="s">
         <v>109</v>
@@ -5534,25 +5514,25 @@
         <v>6</v>
       </c>
       <c r="I116" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J116" t="s">
         <v>117</v>
       </c>
       <c r="K116" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q116" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R116" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="117" spans="1:18">
       <c r="B117" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C117" t="s">
         <v>109</v>
@@ -5570,25 +5550,25 @@
         <v>6</v>
       </c>
       <c r="I117" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J117" t="s">
         <v>117</v>
       </c>
       <c r="K117" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q117" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R117" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="118" spans="1:18">
       <c r="B118" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C118" t="s">
         <v>109</v>
@@ -5606,25 +5586,25 @@
         <v>6</v>
       </c>
       <c r="I118" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J118" t="s">
         <v>117</v>
       </c>
       <c r="K118" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q118" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="119" spans="1:18">
       <c r="B119" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C119" t="s">
         <v>109</v>
@@ -5642,25 +5622,25 @@
         <v>6</v>
       </c>
       <c r="I119" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J119" t="s">
         <v>117</v>
       </c>
       <c r="K119" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q119" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R119" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="120" spans="1:18">
       <c r="B120" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C120" t="s">
         <v>109</v>
@@ -5678,25 +5658,25 @@
         <v>6</v>
       </c>
       <c r="I120" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J120" t="s">
         <v>117</v>
       </c>
       <c r="K120" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q120" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R120" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="121" spans="1:18">
       <c r="B121" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C121" t="s">
         <v>109</v>
@@ -5714,25 +5694,25 @@
         <v>6</v>
       </c>
       <c r="I121" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J121" t="s">
         <v>117</v>
       </c>
       <c r="K121" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q121" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R121" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="122" spans="1:18">
       <c r="B122" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C122" t="s">
         <v>109</v>
@@ -5750,25 +5730,25 @@
         <v>6</v>
       </c>
       <c r="I122" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J122" t="s">
         <v>117</v>
       </c>
       <c r="K122" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Q122" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R122" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="123" spans="1:18">
       <c r="B123" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C123" t="s">
         <v>109</v>
@@ -5786,25 +5766,25 @@
         <v>6</v>
       </c>
       <c r="I123" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J123" t="s">
         <v>117</v>
       </c>
       <c r="K123" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q123" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R123" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "coverage"  ,  "resource"  ,  coverage);</v>
       </c>
     </row>
     <row r="124" spans="1:18">
       <c r="B124" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C124" t="s">
         <v>109</v>
@@ -5822,25 +5802,25 @@
         <v>6</v>
       </c>
       <c r="I124" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J124" t="s">
         <v>117</v>
       </c>
       <c r="K124" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q124" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R124" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "coverage"  ,  "resource"  ,  coverage);</v>
       </c>
     </row>
     <row r="125" spans="1:18">
       <c r="B125" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C125" t="s">
         <v>109</v>
@@ -5858,25 +5838,25 @@
         <v>6</v>
       </c>
       <c r="I125" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J125" t="s">
         <v>117</v>
       </c>
       <c r="K125" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q125" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R125" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "coverage"  ,  "resource"  ,  coverage);</v>
       </c>
     </row>
     <row r="126" spans="1:18">
       <c r="B126" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C126" t="s">
         <v>109</v>
@@ -5894,28 +5874,28 @@
         <v>6</v>
       </c>
       <c r="I126" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J126" t="s">
         <v>117</v>
       </c>
       <c r="K126" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q126" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R126" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "coverage"  ,  "resource"  ,  coverage);</v>
       </c>
     </row>
     <row r="127" spans="1:18">
       <c r="A127" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B127" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C127" t="s">
         <v>109</v>
@@ -5939,19 +5919,19 @@
         <v>21</v>
       </c>
       <c r="K127" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q127" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R127" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "search"  ,  "search"  ,  kws);</v>
       </c>
     </row>
     <row r="128" spans="1:18">
       <c r="B128" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C128" t="s">
         <v>109</v>
@@ -5975,19 +5955,19 @@
         <v>21</v>
       </c>
       <c r="K128" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q128" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R128" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "search"  ,  "search"  ,  kws);</v>
       </c>
     </row>
     <row r="129" spans="2:18">
       <c r="B129" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C129" t="s">
         <v>109</v>
@@ -6011,19 +5991,19 @@
         <v>21</v>
       </c>
       <c r="K129" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q129" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R129" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "search"  ,  "search"  ,  kws);</v>
       </c>
     </row>
     <row r="130" spans="2:18">
       <c r="B130" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C130" t="s">
         <v>109</v>
@@ -6047,13 +6027,13 @@
         <v>21</v>
       </c>
       <c r="K130" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="Q130" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R130" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "search"  ,  "search"  ,  kws);</v>
       </c>
     </row>
@@ -6077,25 +6057,25 @@
         <v>6</v>
       </c>
       <c r="I131" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J131" t="s">
         <v>21</v>
       </c>
       <c r="K131" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q131" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R131" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="132" spans="2:18">
       <c r="B132" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C132" t="s">
         <v>109</v>
@@ -6113,25 +6093,25 @@
         <v>6</v>
       </c>
       <c r="I132" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J132" t="s">
         <v>21</v>
       </c>
       <c r="K132" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q132" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R132" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="133" spans="2:18">
       <c r="B133" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C133" t="s">
         <v>109</v>
@@ -6149,25 +6129,25 @@
         <v>6</v>
       </c>
       <c r="I133" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J133" t="s">
         <v>21</v>
       </c>
       <c r="K133" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q133" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R133" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="134" spans="2:18">
       <c r="B134" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C134" t="s">
         <v>109</v>
@@ -6185,25 +6165,25 @@
         <v>6</v>
       </c>
       <c r="I134" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="J134" t="s">
         <v>21</v>
       </c>
       <c r="K134" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q134" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R134" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="135" spans="2:18">
       <c r="B135" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C135" t="s">
         <v>109</v>
@@ -6221,25 +6201,25 @@
         <v>6</v>
       </c>
       <c r="I135" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J135" t="s">
         <v>21</v>
       </c>
       <c r="K135" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q135" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R135" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="136" spans="2:18">
       <c r="B136" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C136" t="s">
         <v>109</v>
@@ -6257,25 +6237,25 @@
         <v>6</v>
       </c>
       <c r="I136" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J136" t="s">
         <v>21</v>
       </c>
       <c r="K136" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q136" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R136" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="137" spans="2:18">
       <c r="B137" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C137" t="s">
         <v>109</v>
@@ -6293,25 +6273,25 @@
         <v>6</v>
       </c>
       <c r="I137" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J137" t="s">
         <v>21</v>
       </c>
       <c r="K137" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q137" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R137" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="138" spans="2:18">
       <c r="B138" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C138" t="s">
         <v>109</v>
@@ -6329,25 +6309,25 @@
         <v>6</v>
       </c>
       <c r="I138" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J138" t="s">
         <v>21</v>
       </c>
       <c r="K138" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="Q138" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R138" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
       </c>
     </row>
     <row r="139" spans="2:18">
       <c r="B139" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C139" t="s">
         <v>109</v>
@@ -6377,13 +6357,13 @@
         <v>25</v>
       </c>
       <c r="R139" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "city"  ,  "search"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="140" spans="2:18">
       <c r="B140" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C140" t="s">
         <v>109</v>
@@ -6413,13 +6393,13 @@
         <v>25</v>
       </c>
       <c r="R140" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "city"  ,  "search"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="141" spans="2:18">
       <c r="B141" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C141" t="s">
         <v>109</v>
@@ -6449,13 +6429,13 @@
         <v>25</v>
       </c>
       <c r="R141" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "city"  ,  "search"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="142" spans="2:18">
       <c r="B142" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C142" t="s">
         <v>109</v>
@@ -6485,13 +6465,13 @@
         <v>25</v>
       </c>
       <c r="R142" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "city"  ,  "search"  ,  cid.ToString());</v>
       </c>
     </row>
     <row r="143" spans="2:18">
       <c r="B143" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C143" t="s">
         <v>109</v>
@@ -6521,13 +6501,13 @@
         <v>25</v>
       </c>
       <c r="R143" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "province"  ,  "search"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="144" spans="2:18">
       <c r="B144" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C144" t="s">
         <v>109</v>
@@ -6557,13 +6537,13 @@
         <v>25</v>
       </c>
       <c r="R144" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "province"  ,  "search"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="145" spans="2:18">
       <c r="B145" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C145" t="s">
         <v>109</v>
@@ -6593,13 +6573,13 @@
         <v>25</v>
       </c>
       <c r="R145" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "province"  ,  "search"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="146" spans="2:18">
       <c r="B146" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C146" t="s">
         <v>109</v>
@@ -6629,13 +6609,13 @@
         <v>25</v>
       </c>
       <c r="R146" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "province"  ,  "search"  ,  pid.ToString());</v>
       </c>
     </row>
     <row r="147" spans="2:18">
       <c r="B147" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C147" t="s">
         <v>109</v>
@@ -6653,7 +6633,7 @@
         <v>6</v>
       </c>
       <c r="I147" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J147" t="s">
         <v>21</v>
@@ -6665,13 +6645,13 @@
         <v>25</v>
       </c>
       <c r="R147" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "subcategory"  ,  "search"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="148" spans="2:18">
       <c r="B148" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C148" t="s">
         <v>109</v>
@@ -6689,7 +6669,7 @@
         <v>6</v>
       </c>
       <c r="I148" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J148" t="s">
         <v>21</v>
@@ -6701,13 +6681,13 @@
         <v>25</v>
       </c>
       <c r="R148" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "subcategory"  ,  "search"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="149" spans="2:18">
       <c r="B149" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C149" t="s">
         <v>109</v>
@@ -6725,7 +6705,7 @@
         <v>6</v>
       </c>
       <c r="I149" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J149" t="s">
         <v>21</v>
@@ -6737,13 +6717,13 @@
         <v>25</v>
       </c>
       <c r="R149" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "subcategory"  ,  "search"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="150" spans="2:18">
       <c r="B150" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C150" t="s">
         <v>109</v>
@@ -6761,7 +6741,7 @@
         <v>6</v>
       </c>
       <c r="I150" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J150" t="s">
         <v>21</v>
@@ -6773,13 +6753,13 @@
         <v>25</v>
       </c>
       <c r="R150" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "subcategory"  ,  "search"  ,  sid.ToString());</v>
       </c>
     </row>
     <row r="151" spans="2:18">
       <c r="B151" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C151" t="s">
         <v>109</v>
@@ -6797,7 +6777,7 @@
         <v>6</v>
       </c>
       <c r="I151" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="J151" t="s">
         <v>21</v>
@@ -6809,13 +6789,13 @@
         <v>25</v>
       </c>
       <c r="R151" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "topcategory"  ,  "search"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="152" spans="2:18">
       <c r="B152" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C152" t="s">
         <v>109</v>
@@ -6833,7 +6813,7 @@
         <v>6</v>
       </c>
       <c r="I152" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="J152" t="s">
         <v>21</v>
@@ -6845,13 +6825,13 @@
         <v>25</v>
       </c>
       <c r="R152" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "topcategory"  ,  "search"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="153" spans="2:18">
       <c r="B153" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C153" t="s">
         <v>109</v>
@@ -6869,7 +6849,7 @@
         <v>6</v>
       </c>
       <c r="I153" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="J153" t="s">
         <v>21</v>
@@ -6881,13 +6861,13 @@
         <v>25</v>
       </c>
       <c r="R153" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "topcategory"  ,  "search"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="154" spans="2:18">
       <c r="B154" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C154" t="s">
         <v>109</v>
@@ -6905,7 +6885,7 @@
         <v>6</v>
       </c>
       <c r="I154" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="J154" t="s">
         <v>21</v>
@@ -6917,13 +6897,13 @@
         <v>25</v>
       </c>
       <c r="R154" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "topcategory"  ,  "search"  ,  tid.ToString());</v>
       </c>
     </row>
     <row r="155" spans="2:18">
       <c r="B155" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C155" t="s">
         <v>109</v>
@@ -6941,7 +6921,7 @@
         <v>105</v>
       </c>
       <c r="I155" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="J155" t="s">
         <v>21</v>
@@ -6953,13 +6933,13 @@
         <v>25</v>
       </c>
       <c r="R155" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "suggest"  ,  "search"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="156" spans="2:18">
       <c r="B156" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C156" t="s">
         <v>109</v>
@@ -6977,7 +6957,7 @@
         <v>105</v>
       </c>
       <c r="I156" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="J156" t="s">
         <v>21</v>
@@ -6989,13 +6969,13 @@
         <v>25</v>
       </c>
       <c r="R156" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "suggest"  ,  "search"  ,  string.Empty);</v>
       </c>
     </row>
     <row r="157" spans="2:18">
       <c r="B157" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C157" t="s">
         <v>109</v>
@@ -7013,7 +6993,7 @@
         <v>105</v>
       </c>
       <c r="I157" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J157" t="s">
         <v>21</v>
@@ -7025,13 +7005,13 @@
         <v>25</v>
       </c>
       <c r="R157" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "search"  ,  sw);</v>
       </c>
     </row>
     <row r="158" spans="2:18">
       <c r="B158" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C158" t="s">
         <v>109</v>
@@ -7049,7 +7029,7 @@
         <v>105</v>
       </c>
       <c r="I158" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J158" t="s">
         <v>21</v>
@@ -7061,13 +7041,13 @@
         <v>25</v>
       </c>
       <c r="R158" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "search"  ,  sw);</v>
       </c>
     </row>
     <row r="159" spans="2:18">
       <c r="B159" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C159" t="s">
         <v>109</v>
@@ -7085,7 +7065,7 @@
         <v>105</v>
       </c>
       <c r="I159" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J159" t="s">
         <v>21</v>
@@ -7097,13 +7077,13 @@
         <v>25</v>
       </c>
       <c r="R159" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "search"  ,  sw);</v>
       </c>
     </row>
     <row r="160" spans="2:18">
       <c r="B160" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C160" t="s">
         <v>109</v>
@@ -7121,7 +7101,7 @@
         <v>105</v>
       </c>
       <c r="I160" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J160" t="s">
         <v>21</v>
@@ -7133,13 +7113,13 @@
         <v>25</v>
       </c>
       <c r="R160" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  string.Empty  ,  string.Empty  ,  "increment"  ,  "search"  ,  sw);</v>
       </c>
     </row>
     <row r="161" spans="2:18">
       <c r="B161" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C161" t="s">
         <v>109</v>
@@ -7157,25 +7137,25 @@
         <v>6</v>
       </c>
       <c r="I161" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J161" t="s">
         <v>21</v>
       </c>
       <c r="K161" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q161" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R161" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "coverage"  ,  "search"  ,  coverage);</v>
       </c>
     </row>
     <row r="162" spans="2:18">
       <c r="B162" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C162" t="s">
         <v>109</v>
@@ -7193,25 +7173,25 @@
         <v>6</v>
       </c>
       <c r="I162" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J162" t="s">
         <v>21</v>
       </c>
       <c r="K162" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q162" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R162" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "coverage"  ,  "search"  ,  coverage);</v>
       </c>
     </row>
     <row r="163" spans="2:18">
       <c r="B163" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C163" t="s">
         <v>109</v>
@@ -7229,25 +7209,25 @@
         <v>6</v>
       </c>
       <c r="I163" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J163" t="s">
         <v>21</v>
       </c>
       <c r="K163" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q163" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R163" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "coverage"  ,  "search"  ,  coverage);</v>
       </c>
     </row>
     <row r="164" spans="2:18">
       <c r="B164" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C164" t="s">
         <v>109</v>
@@ -7265,19 +7245,19 @@
         <v>6</v>
       </c>
       <c r="I164" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J164" t="s">
         <v>21</v>
       </c>
       <c r="K164" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="Q164" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R164" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "coverage"  ,  "search"  ,  coverage);</v>
       </c>
     </row>
@@ -7295,637 +7275,7 @@
         <v>25</v>
       </c>
       <c r="R165" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="166" spans="2:18">
-      <c r="C166" t="s">
-        <v>109</v>
-      </c>
-      <c r="G166" t="s">
-        <v>1</v>
-      </c>
-      <c r="H166" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q166" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R166" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="167" spans="2:18">
-      <c r="C167" t="s">
-        <v>109</v>
-      </c>
-      <c r="G167" t="s">
-        <v>1</v>
-      </c>
-      <c r="H167" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q167" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R167" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="168" spans="2:18">
-      <c r="C168" t="s">
-        <v>109</v>
-      </c>
-      <c r="G168" t="s">
-        <v>1</v>
-      </c>
-      <c r="H168" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q168" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R168" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="169" spans="2:18">
-      <c r="C169" t="s">
-        <v>109</v>
-      </c>
-      <c r="G169" t="s">
-        <v>1</v>
-      </c>
-      <c r="H169" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q169" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R169" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="170" spans="2:18">
-      <c r="C170" t="s">
-        <v>109</v>
-      </c>
-      <c r="G170" t="s">
-        <v>1</v>
-      </c>
-      <c r="H170" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q170" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R170" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="171" spans="2:18">
-      <c r="C171" t="s">
-        <v>109</v>
-      </c>
-      <c r="G171" t="s">
-        <v>1</v>
-      </c>
-      <c r="H171" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q171" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R171" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="172" spans="2:18">
-      <c r="C172" t="s">
-        <v>109</v>
-      </c>
-      <c r="G172" t="s">
-        <v>1</v>
-      </c>
-      <c r="H172" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q172" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R172" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="173" spans="2:18">
-      <c r="C173" t="s">
-        <v>109</v>
-      </c>
-      <c r="G173" t="s">
-        <v>1</v>
-      </c>
-      <c r="H173" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q173" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R173" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="174" spans="2:18">
-      <c r="C174" t="s">
-        <v>109</v>
-      </c>
-      <c r="G174" t="s">
-        <v>1</v>
-      </c>
-      <c r="H174" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q174" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R174" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="175" spans="2:18">
-      <c r="C175" t="s">
-        <v>109</v>
-      </c>
-      <c r="G175" t="s">
-        <v>1</v>
-      </c>
-      <c r="H175" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q175" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R175" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="176" spans="2:18">
-      <c r="C176" t="s">
-        <v>109</v>
-      </c>
-      <c r="G176" t="s">
-        <v>1</v>
-      </c>
-      <c r="H176" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q176" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R176" t="str">
-        <f t="shared" si="9"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="177" spans="3:18">
-      <c r="C177" t="s">
-        <v>109</v>
-      </c>
-      <c r="G177" t="s">
-        <v>1</v>
-      </c>
-      <c r="H177" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q177" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R177" t="str">
-        <f t="shared" ref="R177:R200" si="10">"logservices.logservices(request, response"&amp;$A$1&amp;C177&amp;$A$1&amp;E177&amp;$A$1&amp;F177&amp;$A$1&amp;G177&amp;$A$1&amp;H177&amp;$A$1&amp;I177&amp;$A$1&amp;J177&amp;$A$1&amp;K177&amp;Q177</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="178" spans="3:18">
-      <c r="C178" t="s">
-        <v>109</v>
-      </c>
-      <c r="G178" t="s">
-        <v>1</v>
-      </c>
-      <c r="H178" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q178" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R178" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="179" spans="3:18">
-      <c r="C179" t="s">
-        <v>109</v>
-      </c>
-      <c r="G179" t="s">
-        <v>1</v>
-      </c>
-      <c r="H179" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q179" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R179" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="180" spans="3:18">
-      <c r="C180" t="s">
-        <v>109</v>
-      </c>
-      <c r="G180" t="s">
-        <v>1</v>
-      </c>
-      <c r="H180" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q180" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R180" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="181" spans="3:18">
-      <c r="C181" t="s">
-        <v>109</v>
-      </c>
-      <c r="G181" t="s">
-        <v>1</v>
-      </c>
-      <c r="H181" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q181" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R181" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="182" spans="3:18">
-      <c r="C182" t="s">
-        <v>109</v>
-      </c>
-      <c r="G182" t="s">
-        <v>1</v>
-      </c>
-      <c r="H182" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q182" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R182" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="183" spans="3:18">
-      <c r="C183" t="s">
-        <v>109</v>
-      </c>
-      <c r="G183" t="s">
-        <v>1</v>
-      </c>
-      <c r="H183" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q183" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R183" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="184" spans="3:18">
-      <c r="C184" t="s">
-        <v>109</v>
-      </c>
-      <c r="G184" t="s">
-        <v>1</v>
-      </c>
-      <c r="H184" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q184" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R184" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="185" spans="3:18">
-      <c r="C185" t="s">
-        <v>109</v>
-      </c>
-      <c r="G185" t="s">
-        <v>1</v>
-      </c>
-      <c r="H185" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q185" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R185" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="186" spans="3:18">
-      <c r="C186" t="s">
-        <v>109</v>
-      </c>
-      <c r="G186" t="s">
-        <v>1</v>
-      </c>
-      <c r="H186" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q186" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R186" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="187" spans="3:18">
-      <c r="C187" t="s">
-        <v>109</v>
-      </c>
-      <c r="G187" t="s">
-        <v>1</v>
-      </c>
-      <c r="H187" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q187" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R187" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="188" spans="3:18">
-      <c r="C188" t="s">
-        <v>109</v>
-      </c>
-      <c r="G188" t="s">
-        <v>1</v>
-      </c>
-      <c r="H188" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q188" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R188" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="189" spans="3:18">
-      <c r="C189" t="s">
-        <v>109</v>
-      </c>
-      <c r="G189" t="s">
-        <v>1</v>
-      </c>
-      <c r="H189" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q189" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R189" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="190" spans="3:18">
-      <c r="C190" t="s">
-        <v>109</v>
-      </c>
-      <c r="G190" t="s">
-        <v>1</v>
-      </c>
-      <c r="H190" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q190" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R190" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="191" spans="3:18">
-      <c r="C191" t="s">
-        <v>109</v>
-      </c>
-      <c r="G191" t="s">
-        <v>1</v>
-      </c>
-      <c r="H191" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q191" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R191" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="192" spans="3:18">
-      <c r="C192" t="s">
-        <v>109</v>
-      </c>
-      <c r="G192" t="s">
-        <v>1</v>
-      </c>
-      <c r="H192" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q192" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R192" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="193" spans="3:18">
-      <c r="C193" t="s">
-        <v>109</v>
-      </c>
-      <c r="G193" t="s">
-        <v>1</v>
-      </c>
-      <c r="H193" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q193" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R193" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="194" spans="3:18">
-      <c r="C194" t="s">
-        <v>109</v>
-      </c>
-      <c r="G194" t="s">
-        <v>1</v>
-      </c>
-      <c r="H194" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q194" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R194" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="195" spans="3:18">
-      <c r="C195" t="s">
-        <v>109</v>
-      </c>
-      <c r="G195" t="s">
-        <v>1</v>
-      </c>
-      <c r="H195" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q195" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R195" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="196" spans="3:18">
-      <c r="C196" t="s">
-        <v>109</v>
-      </c>
-      <c r="G196" t="s">
-        <v>1</v>
-      </c>
-      <c r="H196" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q196" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R196" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="197" spans="3:18">
-      <c r="C197" t="s">
-        <v>109</v>
-      </c>
-      <c r="G197" t="s">
-        <v>1</v>
-      </c>
-      <c r="H197" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q197" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R197" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="198" spans="3:18">
-      <c r="C198" t="s">
-        <v>109</v>
-      </c>
-      <c r="G198" t="s">
-        <v>1</v>
-      </c>
-      <c r="H198" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q198" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R198" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="199" spans="3:18">
-      <c r="C199" t="s">
-        <v>109</v>
-      </c>
-      <c r="G199" t="s">
-        <v>1</v>
-      </c>
-      <c r="H199" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q199" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R199" t="str">
-        <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
-      </c>
-    </row>
-    <row r="200" spans="3:18">
-      <c r="C200" t="s">
-        <v>109</v>
-      </c>
-      <c r="G200" t="s">
-        <v>1</v>
-      </c>
-      <c r="H200" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q200" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R200" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="R165" si="11">"logservices.logservices(request, response"&amp;$A$1&amp;C165&amp;$A$1&amp;E165&amp;$A$1&amp;F165&amp;$A$1&amp;G165&amp;$A$1&amp;H165&amp;$A$1&amp;I165&amp;$A$1&amp;J165&amp;$A$1&amp;K165&amp;Q165</f>
         <v>logservices.logservices(request, response  ,  "dbo"  ,    ,    ,  lang  ,  token  ,    ,    ,  );</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed log keywords string format
</commit_message>
<xml_diff>
--- a/SQLScript/Logfile_info.xlsx
+++ b/SQLScript/Logfile_info.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="284">
   <si>
     <t>csmethod</t>
   </si>
@@ -678,9 +678,6 @@
     <t>"unique"</t>
   </si>
   <si>
-    <t>tid+lang+ran+map+sid</t>
-  </si>
-  <si>
     <t>GetUniqueResources_QS</t>
   </si>
   <si>
@@ -825,12 +822,6 @@
     <t>"circular"</t>
   </si>
   <si>
-    <t>lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString()</t>
-  </si>
-  <si>
-    <t>"lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString()</t>
-  </si>
-  <si>
     <t>GetResourcesInRadiusList_QS</t>
   </si>
   <si>
@@ -904,6 +895,12 @@
   </si>
   <si>
     <t>"Provincal"</t>
+  </si>
+  <si>
+    <t>tid+"/"+lang+"/"+ran+"/"+map+"/"+sid</t>
+  </si>
+  <si>
+    <t>lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString()</t>
   </si>
 </sst>
 </file>
@@ -1297,10 +1294,10 @@
   <dimension ref="A1:T165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B147" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I125" sqref="I125:I126"/>
+      <selection pane="bottomRight" activeCell="K154" sqref="K154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2873,7 +2870,7 @@
         <v>6</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>29</v>
@@ -2909,7 +2906,7 @@
         <v>6</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>29</v>
@@ -2945,7 +2942,7 @@
         <v>6</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>29</v>
@@ -2981,7 +2978,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>29</v>
@@ -3290,7 +3287,7 @@
         <v>167</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>104</v>
@@ -3299,10 +3296,10 @@
         <v>104</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>104</v>
@@ -3314,7 +3311,7 @@
         <v>87</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>25</v>
@@ -3326,7 +3323,7 @@
     </row>
     <row r="56" spans="1:18">
       <c r="B56" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>104</v>
@@ -3335,7 +3332,7 @@
         <v>104</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G56" t="s">
         <v>1</v>
@@ -3347,10 +3344,10 @@
         <v>90</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K56" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q56" s="3" t="s">
         <v>25</v>
@@ -3362,16 +3359,16 @@
     </row>
     <row r="57" spans="1:18">
       <c r="B57" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="G57" t="s">
         <v>1</v>
@@ -3383,10 +3380,10 @@
         <v>90</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q57" s="3" t="s">
         <v>25</v>
@@ -3398,7 +3395,7 @@
     </row>
     <row r="58" spans="1:18">
       <c r="B58" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>104</v>
@@ -3407,10 +3404,10 @@
         <v>104</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>104</v>
@@ -3422,7 +3419,7 @@
         <v>95</v>
       </c>
       <c r="K58" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q58" s="3" t="s">
         <v>25</v>
@@ -3551,7 +3548,7 @@
     </row>
     <row r="62" spans="1:18" s="6" customFormat="1">
       <c r="B62" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C62" t="s">
         <v>109</v>
@@ -3605,7 +3602,7 @@
         <v>104</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>67</v>
@@ -3623,7 +3620,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="B64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C64" t="s">
         <v>109</v>
@@ -3641,7 +3638,7 @@
         <v>104</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>67</v>
@@ -3659,7 +3656,7 @@
     </row>
     <row r="65" spans="1:18">
       <c r="B65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C65" t="s">
         <v>109</v>
@@ -3677,7 +3674,7 @@
         <v>104</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J65" s="6" t="s">
         <v>67</v>
@@ -3695,7 +3692,7 @@
     </row>
     <row r="66" spans="1:18">
       <c r="B66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s">
         <v>109</v>
@@ -3713,7 +3710,7 @@
         <v>104</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J66" s="6" t="s">
         <v>67</v>
@@ -3767,7 +3764,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="B68" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C68" t="s">
         <v>109</v>
@@ -3803,7 +3800,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="B69" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C69" t="s">
         <v>109</v>
@@ -3839,7 +3836,7 @@
     </row>
     <row r="70" spans="1:18">
       <c r="B70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C70" t="s">
         <v>109</v>
@@ -3911,7 +3908,7 @@
     </row>
     <row r="72" spans="1:18">
       <c r="B72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C72" t="s">
         <v>109</v>
@@ -3947,7 +3944,7 @@
     </row>
     <row r="73" spans="1:18">
       <c r="B73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C73" t="s">
         <v>109</v>
@@ -3983,7 +3980,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="B74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C74" t="s">
         <v>109</v>
@@ -4623,19 +4620,19 @@
         <v>117</v>
       </c>
       <c r="K91" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R91" t="str">
         <f>"logservices.logservices(request, response"&amp;$A$1&amp;C91&amp;$A$1&amp;E91&amp;$A$1&amp;F91&amp;$A$1&amp;G91&amp;$A$1&amp;H91&amp;$A$1&amp;I91&amp;$A$1&amp;J91&amp;$A$1&amp;K91&amp;Q91</f>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+"/"+lang+"/"+ran+"/"+map+"/"+sid);</v>
       </c>
     </row>
     <row r="92" spans="2:18">
       <c r="B92" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C92" t="s">
         <v>109</v>
@@ -4659,19 +4656,19 @@
         <v>117</v>
       </c>
       <c r="K92" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="Q92" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R92" t="str">
         <f t="shared" si="8"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+"/"+lang+"/"+ran+"/"+map+"/"+sid);</v>
       </c>
     </row>
     <row r="93" spans="2:18">
       <c r="B93" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C93" t="s">
         <v>109</v>
@@ -4695,19 +4692,19 @@
         <v>117</v>
       </c>
       <c r="K93" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="Q93" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R93" t="str">
         <f t="shared" si="8"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+"/"+lang+"/"+ran+"/"+map+"/"+sid);</v>
       </c>
     </row>
     <row r="94" spans="2:18">
       <c r="B94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C94" t="s">
         <v>109</v>
@@ -4731,19 +4728,19 @@
         <v>117</v>
       </c>
       <c r="K94" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="Q94" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R94" t="str">
         <f t="shared" si="8"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+lang+ran+map+sid);</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "unique"  ,  "resource"  ,  tid+"/"+lang+"/"+ran+"/"+map+"/"+sid);</v>
       </c>
     </row>
     <row r="95" spans="2:18">
       <c r="B95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C95" t="s">
         <v>109</v>
@@ -4761,7 +4758,7 @@
         <v>6</v>
       </c>
       <c r="I95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J95" t="s">
         <v>117</v>
@@ -4779,7 +4776,7 @@
     </row>
     <row r="96" spans="2:18">
       <c r="B96" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C96" t="s">
         <v>109</v>
@@ -4797,7 +4794,7 @@
         <v>6</v>
       </c>
       <c r="I96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J96" t="s">
         <v>117</v>
@@ -4815,7 +4812,7 @@
     </row>
     <row r="97" spans="2:18">
       <c r="B97" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C97" t="s">
         <v>109</v>
@@ -4833,7 +4830,7 @@
         <v>6</v>
       </c>
       <c r="I97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J97" t="s">
         <v>117</v>
@@ -4851,7 +4848,7 @@
     </row>
     <row r="98" spans="2:18">
       <c r="B98" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C98" t="s">
         <v>109</v>
@@ -4869,7 +4866,7 @@
         <v>6</v>
       </c>
       <c r="I98" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J98" t="s">
         <v>117</v>
@@ -4887,7 +4884,7 @@
     </row>
     <row r="99" spans="2:18">
       <c r="B99" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C99" t="s">
         <v>109</v>
@@ -4923,7 +4920,7 @@
     </row>
     <row r="100" spans="2:18">
       <c r="B100" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C100" t="s">
         <v>109</v>
@@ -4959,7 +4956,7 @@
     </row>
     <row r="101" spans="2:18">
       <c r="B101" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C101" t="s">
         <v>109</v>
@@ -4995,7 +4992,7 @@
     </row>
     <row r="102" spans="2:18">
       <c r="B102" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
@@ -5028,7 +5025,7 @@
     </row>
     <row r="103" spans="2:18">
       <c r="B103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C103" t="s">
         <v>109</v>
@@ -5064,7 +5061,7 @@
     </row>
     <row r="104" spans="2:18">
       <c r="B104" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C104" t="s">
         <v>109</v>
@@ -5100,7 +5097,7 @@
     </row>
     <row r="105" spans="2:18">
       <c r="B105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C105" t="s">
         <v>109</v>
@@ -5136,7 +5133,7 @@
     </row>
     <row r="106" spans="2:18">
       <c r="B106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C106" t="s">
         <v>109</v>
@@ -5172,7 +5169,7 @@
     </row>
     <row r="107" spans="2:18">
       <c r="B107" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C107" t="s">
         <v>109</v>
@@ -5208,7 +5205,7 @@
     </row>
     <row r="108" spans="2:18">
       <c r="B108" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C108" t="s">
         <v>109</v>
@@ -5244,7 +5241,7 @@
     </row>
     <row r="109" spans="2:18">
       <c r="B109" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C109" t="s">
         <v>109</v>
@@ -5280,7 +5277,7 @@
     </row>
     <row r="110" spans="2:18">
       <c r="B110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C110" t="s">
         <v>109</v>
@@ -5316,7 +5313,7 @@
     </row>
     <row r="111" spans="2:18">
       <c r="B111" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C111" t="s">
         <v>109</v>
@@ -5340,7 +5337,7 @@
         <v>117</v>
       </c>
       <c r="K111" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q111" s="3" t="s">
         <v>25</v>
@@ -5352,7 +5349,7 @@
     </row>
     <row r="112" spans="2:18">
       <c r="B112" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C112" t="s">
         <v>109</v>
@@ -5376,7 +5373,7 @@
         <v>117</v>
       </c>
       <c r="K112" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q112" s="3" t="s">
         <v>25</v>
@@ -5388,7 +5385,7 @@
     </row>
     <row r="113" spans="1:18">
       <c r="B113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C113" t="s">
         <v>109</v>
@@ -5412,7 +5409,7 @@
         <v>117</v>
       </c>
       <c r="K113" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q113" s="3" t="s">
         <v>25</v>
@@ -5424,7 +5421,7 @@
     </row>
     <row r="114" spans="1:18">
       <c r="B114" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C114" t="s">
         <v>109</v>
@@ -5448,7 +5445,7 @@
         <v>117</v>
       </c>
       <c r="K114" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q114" s="3" t="s">
         <v>25</v>
@@ -5478,25 +5475,25 @@
         <v>6</v>
       </c>
       <c r="I115" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J115" t="s">
         <v>117</v>
       </c>
       <c r="K115" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q115" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R115" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="116" spans="1:18">
       <c r="B116" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C116" t="s">
         <v>109</v>
@@ -5514,25 +5511,25 @@
         <v>6</v>
       </c>
       <c r="I116" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J116" t="s">
         <v>117</v>
       </c>
       <c r="K116" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q116" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R116" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="117" spans="1:18">
       <c r="B117" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C117" t="s">
         <v>109</v>
@@ -5550,25 +5547,25 @@
         <v>6</v>
       </c>
       <c r="I117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J117" t="s">
         <v>117</v>
       </c>
       <c r="K117" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q117" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R117" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="118" spans="1:18">
       <c r="B118" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C118" t="s">
         <v>109</v>
@@ -5586,25 +5583,25 @@
         <v>6</v>
       </c>
       <c r="I118" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J118" t="s">
         <v>117</v>
       </c>
       <c r="K118" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q118" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R118" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="119" spans="1:18">
       <c r="B119" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C119" t="s">
         <v>109</v>
@@ -5622,25 +5619,25 @@
         <v>6</v>
       </c>
       <c r="I119" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J119" t="s">
         <v>117</v>
       </c>
       <c r="K119" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q119" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R119" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="120" spans="1:18">
       <c r="B120" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C120" t="s">
         <v>109</v>
@@ -5658,25 +5655,25 @@
         <v>6</v>
       </c>
       <c r="I120" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J120" t="s">
         <v>117</v>
       </c>
       <c r="K120" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q120" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R120" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="121" spans="1:18">
       <c r="B121" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C121" t="s">
         <v>109</v>
@@ -5694,25 +5691,25 @@
         <v>6</v>
       </c>
       <c r="I121" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J121" t="s">
         <v>117</v>
       </c>
       <c r="K121" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q121" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R121" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="122" spans="1:18">
       <c r="B122" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C122" t="s">
         <v>109</v>
@@ -5730,25 +5727,25 @@
         <v>6</v>
       </c>
       <c r="I122" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J122" t="s">
         <v>117</v>
       </c>
       <c r="K122" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="Q122" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R122" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  "lat"+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "resource"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="123" spans="1:18">
       <c r="B123" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C123" t="s">
         <v>109</v>
@@ -5766,13 +5763,13 @@
         <v>6</v>
       </c>
       <c r="I123" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J123" t="s">
         <v>117</v>
       </c>
       <c r="K123" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q123" s="3" t="s">
         <v>25</v>
@@ -5784,7 +5781,7 @@
     </row>
     <row r="124" spans="1:18">
       <c r="B124" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C124" t="s">
         <v>109</v>
@@ -5802,13 +5799,13 @@
         <v>6</v>
       </c>
       <c r="I124" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J124" t="s">
         <v>117</v>
       </c>
       <c r="K124" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q124" s="3" t="s">
         <v>25</v>
@@ -5820,7 +5817,7 @@
     </row>
     <row r="125" spans="1:18">
       <c r="B125" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C125" t="s">
         <v>109</v>
@@ -5838,13 +5835,13 @@
         <v>6</v>
       </c>
       <c r="I125" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J125" t="s">
         <v>117</v>
       </c>
       <c r="K125" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q125" s="3" t="s">
         <v>25</v>
@@ -5856,7 +5853,7 @@
     </row>
     <row r="126" spans="1:18">
       <c r="B126" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C126" t="s">
         <v>109</v>
@@ -5874,13 +5871,13 @@
         <v>6</v>
       </c>
       <c r="I126" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J126" t="s">
         <v>117</v>
       </c>
       <c r="K126" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q126" s="3" t="s">
         <v>25</v>
@@ -5892,10 +5889,10 @@
     </row>
     <row r="127" spans="1:18">
       <c r="A127" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C127" t="s">
         <v>109</v>
@@ -5919,7 +5916,7 @@
         <v>21</v>
       </c>
       <c r="K127" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q127" s="3" t="s">
         <v>25</v>
@@ -5931,7 +5928,7 @@
     </row>
     <row r="128" spans="1:18">
       <c r="B128" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C128" t="s">
         <v>109</v>
@@ -5955,7 +5952,7 @@
         <v>21</v>
       </c>
       <c r="K128" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q128" s="3" t="s">
         <v>25</v>
@@ -5967,7 +5964,7 @@
     </row>
     <row r="129" spans="2:18">
       <c r="B129" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C129" t="s">
         <v>109</v>
@@ -5991,7 +5988,7 @@
         <v>21</v>
       </c>
       <c r="K129" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q129" s="3" t="s">
         <v>25</v>
@@ -6003,7 +6000,7 @@
     </row>
     <row r="130" spans="2:18">
       <c r="B130" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C130" t="s">
         <v>109</v>
@@ -6027,7 +6024,7 @@
         <v>21</v>
       </c>
       <c r="K130" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q130" s="3" t="s">
         <v>25</v>
@@ -6057,25 +6054,25 @@
         <v>6</v>
       </c>
       <c r="I131" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J131" t="s">
         <v>21</v>
       </c>
       <c r="K131" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q131" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R131" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="132" spans="2:18">
       <c r="B132" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C132" t="s">
         <v>109</v>
@@ -6093,25 +6090,25 @@
         <v>6</v>
       </c>
       <c r="I132" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J132" t="s">
         <v>21</v>
       </c>
       <c r="K132" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q132" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R132" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="133" spans="2:18">
       <c r="B133" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C133" t="s">
         <v>109</v>
@@ -6129,25 +6126,25 @@
         <v>6</v>
       </c>
       <c r="I133" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J133" t="s">
         <v>21</v>
       </c>
       <c r="K133" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q133" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R133" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="134" spans="2:18">
       <c r="B134" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C134" t="s">
         <v>109</v>
@@ -6165,25 +6162,25 @@
         <v>6</v>
       </c>
       <c r="I134" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J134" t="s">
         <v>21</v>
       </c>
       <c r="K134" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q134" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R134" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "circular"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="135" spans="2:18">
       <c r="B135" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C135" t="s">
         <v>109</v>
@@ -6201,25 +6198,25 @@
         <v>6</v>
       </c>
       <c r="I135" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J135" t="s">
         <v>21</v>
       </c>
       <c r="K135" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q135" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R135" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="136" spans="2:18">
       <c r="B136" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C136" t="s">
         <v>109</v>
@@ -6237,25 +6234,25 @@
         <v>6</v>
       </c>
       <c r="I136" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J136" t="s">
         <v>21</v>
       </c>
       <c r="K136" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q136" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R136" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "json"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="137" spans="2:18">
       <c r="B137" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C137" t="s">
         <v>109</v>
@@ -6273,25 +6270,25 @@
         <v>6</v>
       </c>
       <c r="I137" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J137" t="s">
         <v>21</v>
       </c>
       <c r="K137" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q137" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R137" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "path"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="138" spans="2:18">
       <c r="B138" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C138" t="s">
         <v>109</v>
@@ -6309,25 +6306,25 @@
         <v>6</v>
       </c>
       <c r="I138" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J138" t="s">
         <v>21</v>
       </c>
       <c r="K138" t="s">
-        <v>258</v>
+        <v>283</v>
       </c>
       <c r="Q138" s="3" t="s">
         <v>25</v>
       </c>
       <c r="R138" t="str">
         <f t="shared" si="10"/>
-        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat+lat.ToString()+"/lon"+lon.ToString()+"/r"+radius.ToString());</v>
+        <v>logservices.logservices(request, response  ,  "dbo"  ,  "xml"  ,  "query"  ,  lang  ,  token  ,  "box"  ,  "search"  ,  lat.ToString()+"/"+lon.ToString()+"/"+radius.ToString());</v>
       </c>
     </row>
     <row r="139" spans="2:18">
       <c r="B139" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C139" t="s">
         <v>109</v>
@@ -6363,7 +6360,7 @@
     </row>
     <row r="140" spans="2:18">
       <c r="B140" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C140" t="s">
         <v>109</v>
@@ -6399,7 +6396,7 @@
     </row>
     <row r="141" spans="2:18">
       <c r="B141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C141" t="s">
         <v>109</v>
@@ -6435,7 +6432,7 @@
     </row>
     <row r="142" spans="2:18">
       <c r="B142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C142" t="s">
         <v>109</v>
@@ -6471,7 +6468,7 @@
     </row>
     <row r="143" spans="2:18">
       <c r="B143" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C143" t="s">
         <v>109</v>
@@ -6507,7 +6504,7 @@
     </row>
     <row r="144" spans="2:18">
       <c r="B144" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C144" t="s">
         <v>109</v>
@@ -6543,7 +6540,7 @@
     </row>
     <row r="145" spans="2:18">
       <c r="B145" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C145" t="s">
         <v>109</v>
@@ -6579,7 +6576,7 @@
     </row>
     <row r="146" spans="2:18">
       <c r="B146" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C146" t="s">
         <v>109</v>
@@ -6615,7 +6612,7 @@
     </row>
     <row r="147" spans="2:18">
       <c r="B147" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C147" t="s">
         <v>109</v>
@@ -6633,7 +6630,7 @@
         <v>6</v>
       </c>
       <c r="I147" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J147" t="s">
         <v>21</v>
@@ -6651,7 +6648,7 @@
     </row>
     <row r="148" spans="2:18">
       <c r="B148" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C148" t="s">
         <v>109</v>
@@ -6669,7 +6666,7 @@
         <v>6</v>
       </c>
       <c r="I148" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J148" t="s">
         <v>21</v>
@@ -6687,7 +6684,7 @@
     </row>
     <row r="149" spans="2:18">
       <c r="B149" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C149" t="s">
         <v>109</v>
@@ -6705,7 +6702,7 @@
         <v>6</v>
       </c>
       <c r="I149" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J149" t="s">
         <v>21</v>
@@ -6723,7 +6720,7 @@
     </row>
     <row r="150" spans="2:18">
       <c r="B150" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C150" t="s">
         <v>109</v>
@@ -6741,7 +6738,7 @@
         <v>6</v>
       </c>
       <c r="I150" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J150" t="s">
         <v>21</v>
@@ -6759,7 +6756,7 @@
     </row>
     <row r="151" spans="2:18">
       <c r="B151" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C151" t="s">
         <v>109</v>
@@ -6777,7 +6774,7 @@
         <v>6</v>
       </c>
       <c r="I151" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J151" t="s">
         <v>21</v>
@@ -6795,7 +6792,7 @@
     </row>
     <row r="152" spans="2:18">
       <c r="B152" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C152" t="s">
         <v>109</v>
@@ -6813,7 +6810,7 @@
         <v>6</v>
       </c>
       <c r="I152" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J152" t="s">
         <v>21</v>
@@ -6831,7 +6828,7 @@
     </row>
     <row r="153" spans="2:18">
       <c r="B153" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C153" t="s">
         <v>109</v>
@@ -6849,7 +6846,7 @@
         <v>6</v>
       </c>
       <c r="I153" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J153" t="s">
         <v>21</v>
@@ -6867,7 +6864,7 @@
     </row>
     <row r="154" spans="2:18">
       <c r="B154" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C154" t="s">
         <v>109</v>
@@ -6885,7 +6882,7 @@
         <v>6</v>
       </c>
       <c r="I154" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J154" t="s">
         <v>21</v>
@@ -6903,7 +6900,7 @@
     </row>
     <row r="155" spans="2:18">
       <c r="B155" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C155" t="s">
         <v>109</v>
@@ -6921,7 +6918,7 @@
         <v>105</v>
       </c>
       <c r="I155" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J155" t="s">
         <v>21</v>
@@ -6939,7 +6936,7 @@
     </row>
     <row r="156" spans="2:18">
       <c r="B156" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C156" t="s">
         <v>109</v>
@@ -6957,7 +6954,7 @@
         <v>105</v>
       </c>
       <c r="I156" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J156" t="s">
         <v>21</v>
@@ -6975,7 +6972,7 @@
     </row>
     <row r="157" spans="2:18">
       <c r="B157" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C157" t="s">
         <v>109</v>
@@ -7011,7 +7008,7 @@
     </row>
     <row r="158" spans="2:18">
       <c r="B158" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C158" t="s">
         <v>109</v>
@@ -7047,7 +7044,7 @@
     </row>
     <row r="159" spans="2:18">
       <c r="B159" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C159" t="s">
         <v>109</v>
@@ -7083,7 +7080,7 @@
     </row>
     <row r="160" spans="2:18">
       <c r="B160" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C160" t="s">
         <v>109</v>
@@ -7119,7 +7116,7 @@
     </row>
     <row r="161" spans="2:18">
       <c r="B161" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C161" t="s">
         <v>109</v>
@@ -7137,13 +7134,13 @@
         <v>6</v>
       </c>
       <c r="I161" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J161" t="s">
         <v>21</v>
       </c>
       <c r="K161" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q161" s="3" t="s">
         <v>25</v>
@@ -7155,7 +7152,7 @@
     </row>
     <row r="162" spans="2:18">
       <c r="B162" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C162" t="s">
         <v>109</v>
@@ -7173,13 +7170,13 @@
         <v>6</v>
       </c>
       <c r="I162" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J162" t="s">
         <v>21</v>
       </c>
       <c r="K162" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q162" s="3" t="s">
         <v>25</v>
@@ -7191,7 +7188,7 @@
     </row>
     <row r="163" spans="2:18">
       <c r="B163" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C163" t="s">
         <v>109</v>
@@ -7209,13 +7206,13 @@
         <v>6</v>
       </c>
       <c r="I163" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J163" t="s">
         <v>21</v>
       </c>
       <c r="K163" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q163" s="3" t="s">
         <v>25</v>
@@ -7227,7 +7224,7 @@
     </row>
     <row r="164" spans="2:18">
       <c r="B164" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C164" t="s">
         <v>109</v>
@@ -7245,13 +7242,13 @@
         <v>6</v>
       </c>
       <c r="I164" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J164" t="s">
         <v>21</v>
       </c>
       <c r="K164" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Q164" s="3" t="s">
         <v>25</v>

</xml_diff>